<commit_message>
fix mixup with func input
</commit_message>
<xml_diff>
--- a/inputs_outputs.xlsx
+++ b/inputs_outputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\creat_forecast_ad_hoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297D9CD5-C73C-4DF4-BE33-CAF00B2CDBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE7DC40-6CA6-46A7-9146-41D97EA7DBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8928" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8928" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>